<commit_message>
feat: add more llms
</commit_message>
<xml_diff>
--- a/Evaluation/Generation/final_results.xlsx
+++ b/Evaluation/Generation/final_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,15 +479,6 @@
       <c r="P1" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>17</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -497,47 +488,47 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>FinanceBench</t>
+          <t>Table_VQA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>FinanceBench</t>
+          <t>Table_VQA</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>FinanceBench</t>
+          <t>Table_VQA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>FinanceBench</t>
+          <t>Table_VQA</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>FinanceBench</t>
+          <t>Table_VQA</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>FinanceBench</t>
+          <t>Table_VQA</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>FinanceBench</t>
+          <t>Table_VQA</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>FinanceBench</t>
+          <t>Table_VQA</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>FinanceBench</t>
+          <t>Table_VQA</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -566,21 +557,6 @@
         </is>
       </c>
       <c r="P2" t="inlineStr">
-        <is>
-          <t>Table_VQA</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Table_VQA</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Table_VQA</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
         <is>
           <t>Table_VQA</t>
         </is>
@@ -609,75 +585,60 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
           <t>image</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>image</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>image</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>image</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
         <is>
           <t>hybrid</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>hybrid</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>hybrid</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>image</t>
-        </is>
-      </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>image</t>
+          <t>hybrid</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
-        <is>
-          <t>image</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>hybrid</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>hybrid</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
         <is>
           <t>hybrid</t>
         </is>
@@ -706,77 +667,62 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>qwen-25</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>gpt-4o</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>claude</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>google</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>qwen-25</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>gemini-1.5-pro</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>gpt-4o</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>claude</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>google</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>gpt-4o</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>claude</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>google</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>gpt-4o</t>
-        </is>
-      </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>claude</t>
+          <t>qwen-25</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>google</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>gpt-4o</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>claude</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>google</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
     </row>
@@ -787,41 +733,50 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.04666666666666667</v>
+        <v>0.24</v>
       </c>
       <c r="C5" t="n">
-        <v>0.04666666666666667</v>
+        <v>0.224</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01333333333333333</v>
+        <v>0.112</v>
       </c>
       <c r="E5" t="n">
-        <v>0.06081081081081081</v>
+        <v>0.232</v>
       </c>
       <c r="F5" t="n">
-        <v>0.06666666666666667</v>
+        <v>0.124</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01342281879194631</v>
+        <v>0.452</v>
       </c>
       <c r="H5" t="n">
-        <v>0.08</v>
+        <v>0.444</v>
       </c>
       <c r="I5" t="n">
-        <v>0.08</v>
+        <v>0.2409638554216867</v>
       </c>
       <c r="J5" t="n">
-        <v>0.02666666666666667</v>
-      </c>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
+        <v>0.004016064257028112</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.104</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.476</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.504</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.224</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.2530120481927711</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.176</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -830,41 +785,50 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.2516611149784041</v>
+        <v>0.4122325814536341</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2250216946700877</v>
+        <v>0.4548349206349206</v>
       </c>
       <c r="D6" t="n">
-        <v>0.2126499665268905</v>
+        <v>0.3352632622279681</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2572026802583274</v>
+        <v>0.4044222222222222</v>
       </c>
       <c r="F6" t="n">
-        <v>0.2621580133859718</v>
+        <v>0.3475746031746031</v>
       </c>
       <c r="G6" t="n">
-        <v>0.2228389843550961</v>
+        <v>0.7835238095238094</v>
       </c>
       <c r="H6" t="n">
-        <v>0.2989617848244104</v>
+        <v>0.8113142857142857</v>
       </c>
       <c r="I6" t="n">
-        <v>0.279323210966506</v>
+        <v>0.5797956007214092</v>
       </c>
       <c r="J6" t="n">
-        <v>0.2330423909608143</v>
-      </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
+        <v>0.06601644673933831</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.3539272727272727</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.8014545454545455</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.7983437229437229</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.5556857142857143</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.4312009944540065</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.5326666666666666</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -873,84 +837,102 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.1968768161791432</v>
+        <v>0.08043396517781895</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1704241922568116</v>
+        <v>0.09751345912408725</v>
       </c>
       <c r="D7" t="n">
-        <v>0.1912848467596845</v>
+        <v>0.07924119985200585</v>
       </c>
       <c r="E7" t="n">
-        <v>0.191890165398792</v>
+        <v>0.08500407969758361</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1773250029838186</v>
+        <v>0.1026602918901738</v>
       </c>
       <c r="G7" t="n">
-        <v>0.1998777557560704</v>
+        <v>0.1483364357530102</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2104501963274425</v>
+        <v>0.1666057752180688</v>
       </c>
       <c r="I7" t="n">
-        <v>0.1990115470732211</v>
+        <v>0.117876441862915</v>
       </c>
       <c r="J7" t="n">
-        <v>0.1773850903063464</v>
-      </c>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
+        <v>0.03980397267895593</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.1017992816128101</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.09963697991820604</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.1240272302853829</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.08884722823956065</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.06591144205267524</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.09209420530228477</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>G-Eval Mean</t>
+          <t>Bert Score Mean</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.5682417060339403</v>
+        <v>0.6631027999520301</v>
       </c>
       <c r="C8" t="n">
-        <v>0.616896161284071</v>
+        <v>0.6769690741896629</v>
       </c>
       <c r="D8" t="n">
-        <v>0.5469570323142424</v>
+        <v>0.5380090215802192</v>
       </c>
       <c r="E8" t="n">
-        <v>0.5164016364967658</v>
+        <v>0.666713973402977</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5789058055289895</v>
+        <v>0.5734538987874985</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4725970978979958</v>
+        <v>0.8502521013021469</v>
       </c>
       <c r="H8" t="n">
-        <v>0.6152343554057238</v>
+        <v>0.8572390868663787</v>
       </c>
       <c r="I8" t="n">
-        <v>0.6831711012168217</v>
+        <v>0.7117472038450969</v>
       </c>
       <c r="J8" t="n">
-        <v>0.5660077168143975</v>
-      </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
+        <v>0.6062006224470445</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.6983631743192673</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.8581778284311294</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.8664072604179383</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.6925916314125061</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.723248125259656</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.7167851884961128</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: add google flash 2.0 thinking mode
</commit_message>
<xml_diff>
--- a/Evaluation/Generation/final_results.xlsx
+++ b/Evaluation/Generation/final_results.xlsx
@@ -667,62 +667,62 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>qwen-25</t>
+          <t>gemini-1.5-pro</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
+          <t>gemini-2.0-flash-thinking-exp</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>gpt-4o</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>claude</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>google</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
           <t>gemini-1.5-pro</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>gemini-2.0-flash-thinking-exp</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
         <is>
           <t>gpt-4o</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>claude</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>google</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>qwen-25</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>gemini-1.5-pro</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>gpt-4o</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>claude</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>google</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>qwen-25</t>
-        </is>
-      </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>gemini-1.5-pro</t>
+          <t>gemini-2.0-flash-thinking-exp</t>
         </is>
       </c>
     </row>
@@ -742,10 +742,10 @@
         <v>0.112</v>
       </c>
       <c r="E5" t="n">
-        <v>0.232</v>
+        <v>0.124</v>
       </c>
       <c r="F5" t="n">
-        <v>0.124</v>
+        <v>0.1975806451612903</v>
       </c>
       <c r="G5" t="n">
         <v>0.452</v>
@@ -757,10 +757,10 @@
         <v>0.2409638554216867</v>
       </c>
       <c r="J5" t="n">
-        <v>0.004016064257028112</v>
+        <v>0.104</v>
       </c>
       <c r="K5" t="n">
-        <v>0.104</v>
+        <v>0.432</v>
       </c>
       <c r="L5" t="n">
         <v>0.476</v>
@@ -772,10 +772,10 @@
         <v>0.224</v>
       </c>
       <c r="O5" t="n">
-        <v>0.2530120481927711</v>
+        <v>0.176</v>
       </c>
       <c r="P5" t="n">
-        <v>0.176</v>
+        <v>0.4285714285714285</v>
       </c>
     </row>
     <row r="6">
@@ -794,10 +794,10 @@
         <v>0.3352632622279681</v>
       </c>
       <c r="E6" t="n">
-        <v>0.4044222222222222</v>
+        <v>0.3475746031746031</v>
       </c>
       <c r="F6" t="n">
-        <v>0.3475746031746031</v>
+        <v>0.3047566680631197</v>
       </c>
       <c r="G6" t="n">
         <v>0.7835238095238094</v>
@@ -809,10 +809,10 @@
         <v>0.5797956007214092</v>
       </c>
       <c r="J6" t="n">
-        <v>0.06601644673933831</v>
+        <v>0.3539272727272727</v>
       </c>
       <c r="K6" t="n">
-        <v>0.3539272727272727</v>
+        <v>0.6863746031746032</v>
       </c>
       <c r="L6" t="n">
         <v>0.8014545454545455</v>
@@ -824,10 +824,10 @@
         <v>0.5556857142857143</v>
       </c>
       <c r="O6" t="n">
-        <v>0.4312009944540065</v>
+        <v>0.5326666666666666</v>
       </c>
       <c r="P6" t="n">
-        <v>0.5326666666666666</v>
+        <v>0.5608039579468151</v>
       </c>
     </row>
     <row r="7">
@@ -846,10 +846,10 @@
         <v>0.07924119985200585</v>
       </c>
       <c r="E7" t="n">
-        <v>0.08500407969758361</v>
+        <v>0.1026602918901738</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1026602918901738</v>
+        <v>0.07982253108447412</v>
       </c>
       <c r="G7" t="n">
         <v>0.1483364357530102</v>
@@ -861,10 +861,10 @@
         <v>0.117876441862915</v>
       </c>
       <c r="J7" t="n">
-        <v>0.03980397267895593</v>
+        <v>0.1017992816128101</v>
       </c>
       <c r="K7" t="n">
-        <v>0.1017992816128101</v>
+        <v>0.1361237392068599</v>
       </c>
       <c r="L7" t="n">
         <v>0.09963697991820604</v>
@@ -876,10 +876,10 @@
         <v>0.08884722823956065</v>
       </c>
       <c r="O7" t="n">
-        <v>0.06591144205267524</v>
+        <v>0.09209420530228477</v>
       </c>
       <c r="P7" t="n">
-        <v>0.09209420530228477</v>
+        <v>0.08159999192832798</v>
       </c>
     </row>
     <row r="8">
@@ -898,10 +898,10 @@
         <v>0.5380090215802192</v>
       </c>
       <c r="E8" t="n">
-        <v>0.666713973402977</v>
+        <v>0.5734538987874985</v>
       </c>
       <c r="F8" t="n">
-        <v>0.5734538987874985</v>
+        <v>0.589771473720189</v>
       </c>
       <c r="G8" t="n">
         <v>0.8502521013021469</v>
@@ -913,10 +913,10 @@
         <v>0.7117472038450969</v>
       </c>
       <c r="J8" t="n">
-        <v>0.6062006224470445</v>
+        <v>0.6983631743192673</v>
       </c>
       <c r="K8" t="n">
-        <v>0.6983631743192673</v>
+        <v>0.8364856088161469</v>
       </c>
       <c r="L8" t="n">
         <v>0.8581778284311294</v>
@@ -928,10 +928,10 @@
         <v>0.6925916314125061</v>
       </c>
       <c r="O8" t="n">
-        <v>0.723248125259656</v>
+        <v>0.7167851884961128</v>
       </c>
       <c r="P8" t="n">
-        <v>0.7167851884961128</v>
+        <v>0.7471670659829159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: cleanup jsonification of models that doesnt support structured output
</commit_message>
<xml_diff>
--- a/Evaluation/Generation/final_results.xlsx
+++ b/Evaluation/Generation/final_results.xlsx
@@ -775,7 +775,7 @@
         <v>0.176</v>
       </c>
       <c r="P5" t="n">
-        <v>0.4285714285714285</v>
+        <v>0.3870967741935484</v>
       </c>
     </row>
     <row r="6">
@@ -827,7 +827,7 @@
         <v>0.5326666666666666</v>
       </c>
       <c r="P6" t="n">
-        <v>0.5608039579468151</v>
+        <v>0.5355846774193548</v>
       </c>
     </row>
     <row r="7">
@@ -879,7 +879,7 @@
         <v>0.09209420530228477</v>
       </c>
       <c r="P7" t="n">
-        <v>0.08159999192832798</v>
+        <v>0.07949583949697754</v>
       </c>
     </row>
     <row r="8">
@@ -931,7 +931,7 @@
         <v>0.7167851884961128</v>
       </c>
       <c r="P8" t="n">
-        <v>0.7471670659829159</v>
+        <v>0.7384604291930315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>